<commit_message>
updated with latest sabr calibration
</commit_message>
<xml_diff>
--- a/qf605-fixed-income/sabr_calibrated.xlsx
+++ b/qf605-fixed-income/sabr_calibrated.xlsx
@@ -469,19 +469,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.1698556680472279</v>
+        <v>0.1391177694231066</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1815592003308886</v>
+        <v>0.1846311437361156</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1947923220225481</v>
+        <v>0.1968245453932313</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1775474103841898</v>
+        <v>0.1781495538911682</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1717974722663936</v>
+        <v>0.1727589651188632</v>
       </c>
     </row>
     <row r="3">
@@ -491,19 +491,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1130093193447265</v>
+        <v>0.1666405030017211</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1893928179656904</v>
+        <v>0.1986920640478133</v>
       </c>
       <c r="D3" t="n">
-        <v>0.199439168123491</v>
+        <v>0.1999451847614024</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1879044342549528</v>
+        <v>0.1883856878566519</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1713613536164614</v>
+        <v>0.17063106637228</v>
       </c>
     </row>
     <row r="4">
@@ -513,19 +513,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1392457071644742</v>
+        <v>0.1766681763817387</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1579951357236671</v>
+        <v>0.1926930765646341</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1966805550456054</v>
+        <v>0.1965753688622109</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1972117592984672</v>
+        <v>0.1926050870219206</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1794054181588353</v>
+        <v>0.1773786194049607</v>
       </c>
     </row>
   </sheetData>
@@ -581,19 +581,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.5666397869993576</v>
+        <v>-0.6329876681687155</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.5889075463307576</v>
+        <v>-0.525337597569106</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.5208134642629696</v>
+        <v>-0.4831297395439832</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.4342631455290598</v>
+        <v>-0.4165000751703339</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.2939773638822443</v>
+        <v>-0.3080300238788374</v>
       </c>
     </row>
     <row r="3">
@@ -603,19 +603,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.4999766160878332</v>
+        <v>-0.5843784817874683</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.57510020006444</v>
+        <v>-0.5451623032059372</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.5494379677136823</v>
+        <v>-0.5192037559179212</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.5076846131200364</v>
+        <v>-0.498743074072418</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.4017029362689621</v>
+        <v>-0.3901202644965844</v>
       </c>
     </row>
     <row r="4">
@@ -625,19 +625,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.6048359141844176</v>
+        <v>-0.5525023448268775</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.4999999999388394</v>
+        <v>-0.5453249721517903</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.5636619324086403</v>
+        <v>-0.5315120167547526</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.5657386488420222</v>
+        <v>-0.5404873546671907</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.5198018660883619</v>
+        <v>-0.5084018917440672</v>
       </c>
     </row>
   </sheetData>
@@ -693,19 +693,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2.699996814392346</v>
+        <v>2.049198633956934</v>
       </c>
       <c r="C2" t="n">
-        <v>2.293582679143613</v>
+        <v>1.679633689423351</v>
       </c>
       <c r="D2" t="n">
-        <v>1.760673094054363</v>
+        <v>1.441003835359067</v>
       </c>
       <c r="E2" t="n">
-        <v>1.199852824574103</v>
+        <v>1.066331560365873</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8227118726249953</v>
+        <v>0.7699940557453125</v>
       </c>
     </row>
     <row r="3">
@@ -715,19 +715,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.92120700195845</v>
+        <v>1.332680149730216</v>
       </c>
       <c r="C3" t="n">
-        <v>1.375522316946651</v>
+        <v>1.064564699296813</v>
       </c>
       <c r="D3" t="n">
-        <v>1.12734536177372</v>
+        <v>0.953271385366513</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7638607168497515</v>
+        <v>0.6880500324821187</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5737702404812334</v>
+        <v>0.5533080301251064</v>
       </c>
     </row>
     <row r="4">
@@ -737,19 +737,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.634067213694592</v>
+        <v>1.040785710879257</v>
       </c>
       <c r="C4" t="n">
-        <v>1.10904579907918</v>
+        <v>0.9502018101951232</v>
       </c>
       <c r="D4" t="n">
-        <v>1.026228550741676</v>
+        <v>0.8796305578792002</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8035768847332782</v>
+        <v>0.7296450726108302</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6373320404041996</v>
+        <v>0.6199948348583607</v>
       </c>
     </row>
   </sheetData>

</xml_diff>